<commit_message>
Heart Disease / MNIST
</commit_message>
<xml_diff>
--- a/source/08_DeepLearning/data/heart-disease.xlsx
+++ b/source/08_DeepLearning/data/heart-disease.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\big\src\09_ML_DL\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ai\source\08_DeepLearning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249CDB5C-9491-4646-AA31-7F2E9C79B859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27120" yWindow="2460" windowWidth="19356" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="processed.cleveland" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -78,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -701,6 +713,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -736,6 +765,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -911,16 +957,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -964,7 +1013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>63</v>
       </c>
@@ -1008,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>67</v>
       </c>
@@ -1052,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>67</v>
       </c>
@@ -1096,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>37</v>
       </c>
@@ -1140,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>41</v>
       </c>
@@ -1184,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>56</v>
       </c>
@@ -1228,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>62</v>
       </c>
@@ -1272,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>57</v>
       </c>
@@ -1316,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>63</v>
       </c>
@@ -1360,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>53</v>
       </c>
@@ -1404,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>57</v>
       </c>
@@ -1448,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>56</v>
       </c>
@@ -1492,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>56</v>
       </c>
@@ -1536,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>44</v>
       </c>
@@ -1580,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>52</v>
       </c>
@@ -1624,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>57</v>
       </c>
@@ -1668,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>48</v>
       </c>
@@ -1712,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>54</v>
       </c>
@@ -1756,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>48</v>
       </c>
@@ -1800,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>49</v>
       </c>
@@ -1844,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>64</v>
       </c>
@@ -1888,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>58</v>
       </c>
@@ -1932,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>58</v>
       </c>
@@ -1976,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>58</v>
       </c>
@@ -2020,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>60</v>
       </c>
@@ -2064,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>50</v>
       </c>
@@ -2108,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>58</v>
       </c>
@@ -2152,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>66</v>
       </c>
@@ -2196,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>43</v>
       </c>
@@ -2240,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>40</v>
       </c>
@@ -2284,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>69</v>
       </c>
@@ -2328,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>60</v>
       </c>
@@ -2372,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>64</v>
       </c>
@@ -2416,7 +2465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>59</v>
       </c>
@@ -2460,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>44</v>
       </c>
@@ -2504,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>42</v>
       </c>
@@ -2548,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>43</v>
       </c>
@@ -2592,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>57</v>
       </c>
@@ -2636,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>55</v>
       </c>
@@ -2680,7 +2729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>61</v>
       </c>
@@ -2724,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>65</v>
       </c>
@@ -2768,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2812,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>71</v>
       </c>
@@ -2856,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>59</v>
       </c>
@@ -2900,7 +2949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>61</v>
       </c>
@@ -2944,7 +2993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>58</v>
       </c>
@@ -2988,7 +3037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>51</v>
       </c>
@@ -3032,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>50</v>
       </c>
@@ -3076,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>65</v>
       </c>
@@ -3120,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>53</v>
       </c>
@@ -3164,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>41</v>
       </c>
@@ -3208,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>65</v>
       </c>
@@ -3252,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>44</v>
       </c>
@@ -3296,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>44</v>
       </c>
@@ -3340,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>60</v>
       </c>
@@ -3384,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>54</v>
       </c>
@@ -3428,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>50</v>
       </c>
@@ -3472,7 +3521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>41</v>
       </c>
@@ -3516,7 +3565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>54</v>
       </c>
@@ -3560,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>51</v>
       </c>
@@ -3604,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>51</v>
       </c>
@@ -3648,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>46</v>
       </c>
@@ -3692,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>58</v>
       </c>
@@ -3736,7 +3785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>54</v>
       </c>
@@ -3780,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>54</v>
       </c>
@@ -3824,7 +3873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>60</v>
       </c>
@@ -3868,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>60</v>
       </c>
@@ -3912,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>54</v>
       </c>
@@ -3956,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>59</v>
       </c>
@@ -4000,7 +4049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>46</v>
       </c>
@@ -4044,7 +4093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>65</v>
       </c>
@@ -4088,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>67</v>
       </c>
@@ -4132,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>62</v>
       </c>
@@ -4176,7 +4225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>65</v>
       </c>
@@ -4220,7 +4269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>44</v>
       </c>
@@ -4264,7 +4313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>65</v>
       </c>
@@ -4308,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>60</v>
       </c>
@@ -4352,7 +4401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>51</v>
       </c>
@@ -4396,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>48</v>
       </c>
@@ -4440,7 +4489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>58</v>
       </c>
@@ -4484,7 +4533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>45</v>
       </c>
@@ -4528,7 +4577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>53</v>
       </c>
@@ -4572,7 +4621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>39</v>
       </c>
@@ -4616,7 +4665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>68</v>
       </c>
@@ -4660,7 +4709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>52</v>
       </c>
@@ -4704,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>44</v>
       </c>
@@ -4748,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>47</v>
       </c>
@@ -4792,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>53</v>
       </c>
@@ -4836,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>53</v>
       </c>
@@ -4880,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>51</v>
       </c>
@@ -4924,7 +4973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>66</v>
       </c>
@@ -4968,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>62</v>
       </c>
@@ -5012,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>62</v>
       </c>
@@ -5056,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>44</v>
       </c>
@@ -5100,7 +5149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>63</v>
       </c>
@@ -5144,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>52</v>
       </c>
@@ -5188,7 +5237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>59</v>
       </c>
@@ -5232,7 +5281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>60</v>
       </c>
@@ -5276,7 +5325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>52</v>
       </c>
@@ -5320,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>48</v>
       </c>
@@ -5364,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>45</v>
       </c>
@@ -5408,7 +5457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>34</v>
       </c>
@@ -5452,7 +5501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>57</v>
       </c>
@@ -5496,7 +5545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>71</v>
       </c>
@@ -5540,7 +5589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>49</v>
       </c>
@@ -5584,7 +5633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>54</v>
       </c>
@@ -5628,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>59</v>
       </c>
@@ -5672,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>57</v>
       </c>
@@ -5716,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>61</v>
       </c>
@@ -5760,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>39</v>
       </c>
@@ -5804,7 +5853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>61</v>
       </c>
@@ -5848,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>56</v>
       </c>
@@ -5892,7 +5941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>52</v>
       </c>
@@ -5936,7 +5985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>43</v>
       </c>
@@ -5980,7 +6029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>62</v>
       </c>
@@ -6024,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>41</v>
       </c>
@@ -6068,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>58</v>
       </c>
@@ -6112,7 +6161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>35</v>
       </c>
@@ -6156,7 +6205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>63</v>
       </c>
@@ -6200,7 +6249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>65</v>
       </c>
@@ -6244,7 +6293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>48</v>
       </c>
@@ -6288,7 +6337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>63</v>
       </c>
@@ -6332,7 +6381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>51</v>
       </c>
@@ -6376,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>55</v>
       </c>
@@ -6420,7 +6469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>65</v>
       </c>
@@ -6464,7 +6513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>45</v>
       </c>
@@ -6508,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>56</v>
       </c>
@@ -6552,7 +6601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>54</v>
       </c>
@@ -6596,7 +6645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>44</v>
       </c>
@@ -6640,7 +6689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>62</v>
       </c>
@@ -6684,7 +6733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>54</v>
       </c>
@@ -6728,7 +6777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>51</v>
       </c>
@@ -6772,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>29</v>
       </c>
@@ -6816,7 +6865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>51</v>
       </c>
@@ -6860,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>43</v>
       </c>
@@ -6904,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>55</v>
       </c>
@@ -6948,7 +6997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>70</v>
       </c>
@@ -6992,7 +7041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>62</v>
       </c>
@@ -7036,7 +7085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>35</v>
       </c>
@@ -7080,7 +7129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>51</v>
       </c>
@@ -7124,7 +7173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>59</v>
       </c>
@@ -7168,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>59</v>
       </c>
@@ -7212,7 +7261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>52</v>
       </c>
@@ -7256,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>64</v>
       </c>
@@ -7300,7 +7349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>58</v>
       </c>
@@ -7344,7 +7393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>47</v>
       </c>
@@ -7388,7 +7437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>57</v>
       </c>
@@ -7432,7 +7481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>41</v>
       </c>
@@ -7476,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>45</v>
       </c>
@@ -7520,7 +7569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>60</v>
       </c>
@@ -7564,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>52</v>
       </c>
@@ -7608,7 +7657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>42</v>
       </c>
@@ -7652,7 +7701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>67</v>
       </c>
@@ -7696,7 +7745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>55</v>
       </c>
@@ -7740,7 +7789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>64</v>
       </c>
@@ -7784,7 +7833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>70</v>
       </c>
@@ -7828,7 +7877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>51</v>
       </c>
@@ -7872,7 +7921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>58</v>
       </c>
@@ -7916,7 +7965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>60</v>
       </c>
@@ -7960,7 +8009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>68</v>
       </c>
@@ -8004,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>46</v>
       </c>
@@ -8048,7 +8097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>77</v>
       </c>
@@ -8092,7 +8141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>54</v>
       </c>
@@ -8136,7 +8185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>58</v>
       </c>
@@ -8180,7 +8229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>48</v>
       </c>
@@ -8224,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>57</v>
       </c>
@@ -8268,7 +8317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>52</v>
       </c>
@@ -8312,7 +8361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>54</v>
       </c>
@@ -8356,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>35</v>
       </c>
@@ -8400,7 +8449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>45</v>
       </c>
@@ -8444,7 +8493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>70</v>
       </c>
@@ -8488,7 +8537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>53</v>
       </c>
@@ -8532,7 +8581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>59</v>
       </c>
@@ -8576,7 +8625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>62</v>
       </c>
@@ -8620,7 +8669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>64</v>
       </c>
@@ -8664,7 +8713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>57</v>
       </c>
@@ -8708,7 +8757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>52</v>
       </c>
@@ -8752,7 +8801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>56</v>
       </c>
@@ -8796,7 +8845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>43</v>
       </c>
@@ -8840,7 +8889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>53</v>
       </c>
@@ -8884,7 +8933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>48</v>
       </c>
@@ -8928,7 +8977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>56</v>
       </c>
@@ -8972,7 +9021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>42</v>
       </c>
@@ -9016,7 +9065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>59</v>
       </c>
@@ -9060,7 +9109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>60</v>
       </c>
@@ -9104,7 +9153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>63</v>
       </c>
@@ -9148,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>42</v>
       </c>
@@ -9192,7 +9241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>66</v>
       </c>
@@ -9236,7 +9285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>54</v>
       </c>
@@ -9280,7 +9329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>69</v>
       </c>
@@ -9324,7 +9373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>50</v>
       </c>
@@ -9368,7 +9417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>51</v>
       </c>
@@ -9412,7 +9461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>43</v>
       </c>
@@ -9456,7 +9505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>62</v>
       </c>
@@ -9500,7 +9549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>68</v>
       </c>
@@ -9544,7 +9593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>67</v>
       </c>
@@ -9588,7 +9637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>69</v>
       </c>
@@ -9632,7 +9681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>45</v>
       </c>
@@ -9676,7 +9725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>50</v>
       </c>
@@ -9720,7 +9769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>59</v>
       </c>
@@ -9764,7 +9813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>50</v>
       </c>
@@ -9808,7 +9857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>64</v>
       </c>
@@ -9852,7 +9901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>57</v>
       </c>
@@ -9896,7 +9945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>64</v>
       </c>
@@ -9940,7 +9989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>43</v>
       </c>
@@ -9984,7 +10033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>45</v>
       </c>
@@ -10028,7 +10077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>58</v>
       </c>
@@ -10072,7 +10121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>50</v>
       </c>
@@ -10116,7 +10165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>55</v>
       </c>
@@ -10160,7 +10209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>62</v>
       </c>
@@ -10204,7 +10253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>37</v>
       </c>
@@ -10248,7 +10297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>38</v>
       </c>
@@ -10292,7 +10341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>41</v>
       </c>
@@ -10336,7 +10385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>66</v>
       </c>
@@ -10380,7 +10429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>52</v>
       </c>
@@ -10424,7 +10473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>56</v>
       </c>
@@ -10468,7 +10517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>46</v>
       </c>
@@ -10512,7 +10561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>46</v>
       </c>
@@ -10556,7 +10605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>64</v>
       </c>
@@ -10600,7 +10649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>59</v>
       </c>
@@ -10644,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>41</v>
       </c>
@@ -10688,7 +10737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>54</v>
       </c>
@@ -10732,7 +10781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>39</v>
       </c>
@@ -10776,7 +10825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>53</v>
       </c>
@@ -10820,7 +10869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>63</v>
       </c>
@@ -10864,7 +10913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>34</v>
       </c>
@@ -10908,7 +10957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>47</v>
       </c>
@@ -10952,7 +11001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>67</v>
       </c>
@@ -10996,7 +11045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>54</v>
       </c>
@@ -11040,7 +11089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>66</v>
       </c>
@@ -11084,7 +11133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>52</v>
       </c>
@@ -11128,7 +11177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>55</v>
       </c>
@@ -11172,7 +11221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>49</v>
       </c>
@@ -11216,7 +11265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>74</v>
       </c>
@@ -11260,7 +11309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>54</v>
       </c>
@@ -11304,7 +11353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>54</v>
       </c>
@@ -11348,7 +11397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>56</v>
       </c>
@@ -11392,7 +11441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>46</v>
       </c>
@@ -11436,7 +11485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>49</v>
       </c>
@@ -11480,7 +11529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>42</v>
       </c>
@@ -11524,7 +11573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>41</v>
       </c>
@@ -11568,7 +11617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>41</v>
       </c>
@@ -11612,7 +11661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>49</v>
       </c>
@@ -11656,7 +11705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>61</v>
       </c>
@@ -11700,7 +11749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>60</v>
       </c>
@@ -11744,7 +11793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>67</v>
       </c>
@@ -11788,7 +11837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>58</v>
       </c>
@@ -11832,7 +11881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>47</v>
       </c>
@@ -11876,7 +11925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>52</v>
       </c>
@@ -11920,7 +11969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>62</v>
       </c>
@@ -11964,7 +12013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>57</v>
       </c>
@@ -12008,7 +12057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>58</v>
       </c>
@@ -12052,7 +12101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>64</v>
       </c>
@@ -12096,7 +12145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>51</v>
       </c>
@@ -12140,7 +12189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>43</v>
       </c>
@@ -12184,7 +12233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>42</v>
       </c>
@@ -12228,7 +12277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>67</v>
       </c>
@@ -12272,7 +12321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>76</v>
       </c>
@@ -12316,7 +12365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>70</v>
       </c>
@@ -12360,7 +12409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>57</v>
       </c>
@@ -12404,7 +12453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>44</v>
       </c>
@@ -12448,7 +12497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>58</v>
       </c>
@@ -12492,7 +12541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>60</v>
       </c>
@@ -12536,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>44</v>
       </c>
@@ -12580,7 +12629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>61</v>
       </c>
@@ -12624,7 +12673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>42</v>
       </c>
@@ -12668,7 +12717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>52</v>
       </c>
@@ -12712,7 +12761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>59</v>
       </c>
@@ -12756,7 +12805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>40</v>
       </c>
@@ -12800,7 +12849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>42</v>
       </c>
@@ -12844,7 +12893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>61</v>
       </c>
@@ -12888,7 +12937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>66</v>
       </c>
@@ -12932,7 +12981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>46</v>
       </c>
@@ -12976,7 +13025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>71</v>
       </c>
@@ -13020,7 +13069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>59</v>
       </c>
@@ -13064,7 +13113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>64</v>
       </c>
@@ -13108,7 +13157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>66</v>
       </c>
@@ -13152,7 +13201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>39</v>
       </c>
@@ -13196,7 +13245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>57</v>
       </c>
@@ -13240,7 +13289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>58</v>
       </c>
@@ -13284,7 +13333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>57</v>
       </c>
@@ -13328,7 +13377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>47</v>
       </c>
@@ -13372,7 +13421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>55</v>
       </c>
@@ -13416,7 +13465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>35</v>
       </c>
@@ -13460,7 +13509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>61</v>
       </c>
@@ -13504,7 +13553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>58</v>
       </c>
@@ -13548,7 +13597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>58</v>
       </c>
@@ -13592,7 +13641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>58</v>
       </c>
@@ -13636,7 +13685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>56</v>
       </c>
@@ -13680,7 +13729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>56</v>
       </c>
@@ -13724,7 +13773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>67</v>
       </c>
@@ -13768,7 +13817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>55</v>
       </c>
@@ -13812,7 +13861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>44</v>
       </c>
@@ -13856,7 +13905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>63</v>
       </c>
@@ -13900,7 +13949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>63</v>
       </c>
@@ -13944,7 +13993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>41</v>
       </c>
@@ -13988,7 +14037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>59</v>
       </c>
@@ -14032,7 +14081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>57</v>
       </c>
@@ -14076,7 +14125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>45</v>
       </c>
@@ -14120,7 +14169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>68</v>
       </c>
@@ -14164,7 +14213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>57</v>
       </c>
@@ -14208,7 +14257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>57</v>
       </c>
@@ -14252,7 +14301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>38</v>
       </c>

</xml_diff>